<commit_message>
Improvements gemengt und data collected.
</commit_message>
<xml_diff>
--- a/MuS_Data.xlsx
+++ b/MuS_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\ModellierungUndSimulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD38A697-D141-4EAB-99FD-2430D0DDF929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0502AB-AF49-4593-9D50-E1E51AF781ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="12">
   <si>
     <t>LIFO</t>
   </si>
@@ -387,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T51"/>
+  <dimension ref="A1:AC51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="U20" sqref="T20:U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,7 +401,7 @@
     <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -447,8 +447,20 @@
       <c r="T1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA1">
+        <v>2370</v>
+      </c>
+      <c r="AB1">
+        <v>2788</v>
+      </c>
+      <c r="AC1">
+        <v>5158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -494,8 +506,20 @@
       <c r="T2">
         <v>3163</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1873</v>
+      </c>
+      <c r="AB2">
+        <v>2788</v>
+      </c>
+      <c r="AC2">
+        <v>4661</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -541,8 +565,20 @@
       <c r="T3">
         <v>2837</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>2148</v>
+      </c>
+      <c r="AB3">
+        <v>2788</v>
+      </c>
+      <c r="AC3">
+        <v>4937</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -588,8 +624,20 @@
       <c r="T4">
         <v>2811</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA4">
+        <v>2075</v>
+      </c>
+      <c r="AB4">
+        <v>2788</v>
+      </c>
+      <c r="AC4">
+        <v>4864</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -636,7 +684,7 @@
         <v>3093</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -683,7 +731,7 @@
         <v>2953</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -738,7 +786,7 @@
         <v>2971.4</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -755,7 +803,7 @@
         <v>4959</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -778,7 +826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -798,7 +846,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -815,7 +863,7 @@
         <v>4322</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -832,7 +880,7 @@
         <v>4219</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -849,7 +897,7 @@
         <v>4892</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -866,7 +914,7 @@
         <v>4966</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -883,7 +931,7 @@
         <v>5285</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>

</xml_diff>